<commit_message>
Small fix for tomarrow
Original List is correct but other stuff is not need to revise
</commit_message>
<xml_diff>
--- a/Task1.xlsx
+++ b/Task1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rishabhs\Downloads\Interview Task\Task 1 (C#)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/67838df926c0509b/Documents/GitHub/Task1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8A9138-0C5B-49D4-94ED-A3D2DD1CD409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{CD8A9138-0C5B-49D4-94ED-A3D2DD1CD409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D76A9BF6-D8C8-4385-B0CD-383021DA6F32}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6B3F0E5-A980-4F34-862A-4513D529DA68}"/>
+    <workbookView xWindow="8610" yWindow="1185" windowWidth="15240" windowHeight="13575" xr2:uid="{C6B3F0E5-A980-4F34-862A-4513D529DA68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="413">
   <si>
     <t>Line 1</t>
   </si>
@@ -1272,6 +1272,9 @@
   </si>
   <si>
     <t>Label of End Node</t>
+  </si>
+  <si>
+    <t>Line TEST</t>
   </si>
 </sst>
 </file>
@@ -1340,9 +1343,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1380,7 +1383,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1486,7 +1489,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1628,7 +1631,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1636,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E00A463-E224-4D17-B4A2-1644EFD9964A}">
-  <dimension ref="A1:D410"/>
+  <dimension ref="A1:D411"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A400" workbookViewId="0">
+      <selection activeCell="C411" sqref="C411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6569,6 +6572,17 @@
       </c>
       <c r="D410" s="1"/>
     </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A411" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B411" s="2">
+        <v>9999999</v>
+      </c>
+      <c r="C411" s="2">
+        <v>8888888</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D410">
     <sortCondition ref="D2:D410"/>

</xml_diff>